<commit_message>
update IMGT results parser
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92B5F94-63B4-BB41-BA7F-1FC674075AA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E0661B-36F8-0243-8C57-FE177E601336}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20220" yWindow="3380" windowWidth="27300" windowHeight="20760" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="11880" yWindow="6340" windowWidth="27300" windowHeight="20760" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="238">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -736,6 +736,9 @@
   </si>
   <si>
     <t>function</t>
+  </si>
+  <si>
+    <t>6_junction</t>
   </si>
 </sst>
 </file>
@@ -1105,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1CAC7E-D6FA-A445-AE9E-B41AFE7C83FC}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3054,10 +3057,11 @@
       <c r="E77" t="s">
         <v>207</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H77" s="1">
+      <c r="G77" s="2"/>
+      <c r="H77" s="3">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
@@ -3078,10 +3082,11 @@
       <c r="E78" t="s">
         <v>207</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H78" s="1">
+      <c r="G78" s="2"/>
+      <c r="H78" s="3">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
@@ -3102,10 +3107,11 @@
       <c r="E79" t="s">
         <v>207</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="H79" s="1">
+      <c r="G79" s="2"/>
+      <c r="H79" s="3">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
@@ -3598,6 +3604,18 @@
       <c r="C101" t="s">
         <v>176</v>
       </c>
+      <c r="D101" t="s">
+        <v>207</v>
+      </c>
+      <c r="E101" t="s">
+        <v>207</v>
+      </c>
+      <c r="F101" t="s">
+        <v>237</v>
+      </c>
+      <c r="G101">
+        <v>71</v>
+      </c>
       <c r="H101" s="1">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -3613,6 +3631,18 @@
       <c r="C102" t="s">
         <v>178</v>
       </c>
+      <c r="D102" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" t="s">
+        <v>207</v>
+      </c>
+      <c r="F102" t="s">
+        <v>237</v>
+      </c>
+      <c r="G102">
+        <v>72</v>
+      </c>
       <c r="H102" s="1">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3632,7 +3662,10 @@
         <v>207</v>
       </c>
       <c r="E103" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="F103" t="s">
+        <v>236</v>
       </c>
       <c r="H103" s="1">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update IMGT result parser
later need to confirm the germline results with more testing data
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDEBCB9-F798-664D-A279-9768B561C789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D66807-BED0-324D-95DD-CF9F811891C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24280" yWindow="5500" windowWidth="27300" windowHeight="20760" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="15380" yWindow="4800" windowWidth="27300" windowHeight="20760" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="239">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>6_junction</t>
+  </si>
+  <si>
+    <t>6 pr 7</t>
   </si>
 </sst>
 </file>
@@ -787,11 +790,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1CAC7E-D6FA-A445-AE9E-B41AFE7C83FC}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="L81" sqref="L81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1469,6 +1473,12 @@
       <c r="E14" t="s">
         <v>207</v>
       </c>
+      <c r="F14" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H14" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2723,6 +2733,10 @@
         <v>207</v>
       </c>
       <c r="E61" s="1"/>
+      <c r="F61" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G61" s="4"/>
       <c r="H61" s="1">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2742,6 +2756,10 @@
         <v>207</v>
       </c>
       <c r="E62" s="1"/>
+      <c r="F62" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G62" s="4"/>
       <c r="H62" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2761,6 +2779,10 @@
         <v>207</v>
       </c>
       <c r="E63" s="1"/>
+      <c r="F63" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G63" s="4"/>
       <c r="H63" s="1">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2780,6 +2802,10 @@
         <v>207</v>
       </c>
       <c r="E64" s="1"/>
+      <c r="F64" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G64" s="4"/>
       <c r="H64" s="1">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2799,6 +2825,10 @@
         <v>207</v>
       </c>
       <c r="E65" s="1"/>
+      <c r="F65" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G65" s="4"/>
       <c r="H65" s="1">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2818,6 +2848,10 @@
         <v>207</v>
       </c>
       <c r="E66" s="1"/>
+      <c r="F66" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G66" s="4"/>
       <c r="H66" s="1">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2837,6 +2871,10 @@
         <v>207</v>
       </c>
       <c r="E67" s="1"/>
+      <c r="F67" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G67" s="4"/>
       <c r="H67" s="1">
         <f t="shared" ref="H67:H121" si="1">A67-1</f>
         <v>65</v>
@@ -2856,6 +2894,10 @@
         <v>207</v>
       </c>
       <c r="E68" s="1"/>
+      <c r="F68" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G68" s="4"/>
       <c r="H68" s="1">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -3198,8 +3240,8 @@
       <c r="F81" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G81" s="2">
-        <v>5</v>
+      <c r="G81" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="H81" s="3">
         <f t="shared" si="1"/>
@@ -3219,6 +3261,12 @@
       <c r="D82" t="s">
         <v>207</v>
       </c>
+      <c r="E82" t="s">
+        <v>207</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>236</v>
+      </c>
       <c r="H82" s="1">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3601,10 +3649,10 @@
       <c r="F99" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="2">
         <v>4</v>
       </c>
-      <c r="H99" s="1">
+      <c r="H99" s="3">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
@@ -3700,10 +3748,11 @@
       <c r="E103" t="s">
         <v>207</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H103" s="1">
+      <c r="G103" s="2"/>
+      <c r="H103" s="3">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
@@ -3980,5 +4029,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
try to improve result import from IgBlast
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A74E8-85ED-5746-859C-DDC8C55726A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6863D891-5C07-DD4F-9574-ECBC2321449A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="4800" windowWidth="27300" windowHeight="20760" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="15380" yWindow="4800" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IMGT" sheetId="1" r:id="rId1"/>
+    <sheet name="IgBlast" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="266">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -742,6 +743,87 @@
   </si>
   <si>
     <t>6 pr 7</t>
+  </si>
+  <si>
+    <t>IgBlast FMT 19</t>
+  </si>
+  <si>
+    <t>74-62</t>
+  </si>
+  <si>
+    <t>75-62</t>
+  </si>
+  <si>
+    <t>77-62</t>
+  </si>
+  <si>
+    <t>76-62</t>
+  </si>
+  <si>
+    <t>78-62</t>
+  </si>
+  <si>
+    <t>79-62</t>
+  </si>
+  <si>
+    <t>80-62</t>
+  </si>
+  <si>
+    <t>81-62</t>
+  </si>
+  <si>
+    <t>82-62</t>
+  </si>
+  <si>
+    <t>83-62</t>
+  </si>
+  <si>
+    <t>75-74</t>
+  </si>
+  <si>
+    <t>77-76</t>
+  </si>
+  <si>
+    <t>79-78</t>
+  </si>
+  <si>
+    <t>81-80</t>
+  </si>
+  <si>
+    <t>83-82</t>
+  </si>
+  <si>
+    <t>cmp 10 and 11</t>
+  </si>
+  <si>
+    <t>IgBlast FMT 3</t>
+  </si>
+  <si>
+    <t>V-(D)-J junction</t>
+  </si>
+  <si>
+    <t>j begin - v end</t>
+  </si>
+  <si>
+    <t>V-(D)-J rearrangement</t>
+  </si>
+  <si>
+    <t>Alignments</t>
+  </si>
+  <si>
+    <t>cmp 12 and 13</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>j1</t>
   </si>
 </sst>
 </file>
@@ -790,12 +872,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1CAC7E-D6FA-A445-AE9E-B41AFE7C83FC}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98:G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1128,9 +1214,11 @@
       <c r="D1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>209</v>
       </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1" t="s">
         <v>213</v>
       </c>
@@ -3850,6 +3938,9 @@
       <c r="C109" t="s">
         <v>190</v>
       </c>
+      <c r="F109" t="s">
+        <v>156</v>
+      </c>
       <c r="H109" s="1">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -4036,7 +4127,2707 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
+  <dimension ref="A1:H121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f>A2-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G66" si="0">A3-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="4">
+        <v>7</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="4">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F9" s="4">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" s="4">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="4">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="4">
+        <v>9</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="4">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>207</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" t="s">
+        <v>207</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" t="s">
+        <v>210</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>207</v>
+      </c>
+      <c r="E20" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" t="s">
+        <v>210</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" t="s">
+        <v>207</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" t="s">
+        <v>207</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G27" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" t="s">
+        <v>207</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G28" s="3">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>207</v>
+      </c>
+      <c r="E31" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="3">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" t="s">
+        <v>207</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G32" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" t="s">
+        <v>207</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34" t="s">
+        <v>207</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E35" t="s">
+        <v>207</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>207</v>
+      </c>
+      <c r="E36" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" t="s">
+        <v>207</v>
+      </c>
+      <c r="E37" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G37" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38" t="s">
+        <v>207</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" t="s">
+        <v>207</v>
+      </c>
+      <c r="E39" t="s">
+        <v>207</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G39" s="3">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" t="s">
+        <v>207</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G40" s="3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41" t="s">
+        <v>207</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G41" s="3">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" t="s">
+        <v>207</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G42" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" t="s">
+        <v>207</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G43" s="3">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" t="s">
+        <v>207</v>
+      </c>
+      <c r="E44" t="s">
+        <v>207</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G44" s="3">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" t="s">
+        <v>207</v>
+      </c>
+      <c r="E45" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G45" s="3">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>207</v>
+      </c>
+      <c r="E46" t="s">
+        <v>207</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G46" s="3">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>207</v>
+      </c>
+      <c r="E47" t="s">
+        <v>207</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" t="s">
+        <v>207</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" t="s">
+        <v>207</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" t="s">
+        <v>207</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>207</v>
+      </c>
+      <c r="E51" t="s">
+        <v>207</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>207</v>
+      </c>
+      <c r="E52" t="s">
+        <v>207</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>207</v>
+      </c>
+      <c r="E53" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G53" s="3">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>207</v>
+      </c>
+      <c r="E54" t="s">
+        <v>207</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G54" s="3">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" t="s">
+        <v>207</v>
+      </c>
+      <c r="E55" t="s">
+        <v>207</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" t="s">
+        <v>207</v>
+      </c>
+      <c r="E56" t="s">
+        <v>207</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G56" s="3">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" t="s">
+        <v>207</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" t="s">
+        <v>207</v>
+      </c>
+      <c r="E58" t="s">
+        <v>207</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="G58" s="3">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" t="s">
+        <v>207</v>
+      </c>
+      <c r="E59" t="s">
+        <v>207</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G59" s="3">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" t="s">
+        <v>207</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="H60" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" t="s">
+        <v>207</v>
+      </c>
+      <c r="E61" t="s">
+        <v>207</v>
+      </c>
+      <c r="F61" s="4">
+        <v>64</v>
+      </c>
+      <c r="G61" s="3">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" t="s">
+        <v>207</v>
+      </c>
+      <c r="E62" t="s">
+        <v>207</v>
+      </c>
+      <c r="F62" s="4">
+        <v>65</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" t="s">
+        <v>207</v>
+      </c>
+      <c r="E63" t="s">
+        <v>207</v>
+      </c>
+      <c r="F63" s="4">
+        <v>68</v>
+      </c>
+      <c r="G63" s="3">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" t="s">
+        <v>207</v>
+      </c>
+      <c r="E64" t="s">
+        <v>207</v>
+      </c>
+      <c r="F64" s="4">
+        <v>69</v>
+      </c>
+      <c r="G64" s="3">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>118</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" t="s">
+        <v>207</v>
+      </c>
+      <c r="E65" t="s">
+        <v>207</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G65" s="3">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D66" t="s">
+        <v>207</v>
+      </c>
+      <c r="E66" t="s">
+        <v>207</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G66" s="3">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" t="s">
+        <v>123</v>
+      </c>
+      <c r="D67" t="s">
+        <v>207</v>
+      </c>
+      <c r="E67" t="s">
+        <v>207</v>
+      </c>
+      <c r="F67" s="4">
+        <v>72</v>
+      </c>
+      <c r="G67" s="3">
+        <f t="shared" ref="G67:G121" si="1">A67-1</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>124</v>
+      </c>
+      <c r="C68" t="s">
+        <v>125</v>
+      </c>
+      <c r="D68" t="s">
+        <v>207</v>
+      </c>
+      <c r="E68" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" s="4">
+        <v>73</v>
+      </c>
+      <c r="G68" s="3">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" t="s">
+        <v>207</v>
+      </c>
+      <c r="F69" s="4">
+        <v>14</v>
+      </c>
+      <c r="G69" s="3">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" t="s">
+        <v>128</v>
+      </c>
+      <c r="D70" t="s">
+        <v>207</v>
+      </c>
+      <c r="E70" t="s">
+        <v>207</v>
+      </c>
+      <c r="F70" s="4">
+        <v>15</v>
+      </c>
+      <c r="G70" s="3">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" t="s">
+        <v>207</v>
+      </c>
+      <c r="F71" s="4">
+        <v>16</v>
+      </c>
+      <c r="G71" s="3">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" t="s">
+        <v>131</v>
+      </c>
+      <c r="D72" t="s">
+        <v>207</v>
+      </c>
+      <c r="E72" t="s">
+        <v>207</v>
+      </c>
+      <c r="F72" s="4">
+        <v>17</v>
+      </c>
+      <c r="G72" s="3">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" t="s">
+        <v>207</v>
+      </c>
+      <c r="E73" t="s">
+        <v>207</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G73" s="3">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>134</v>
+      </c>
+      <c r="C74" t="s">
+        <v>134</v>
+      </c>
+      <c r="D74" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" t="s">
+        <v>207</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G74" s="3">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" t="s">
+        <v>207</v>
+      </c>
+      <c r="E75" t="s">
+        <v>207</v>
+      </c>
+      <c r="F75" s="4">
+        <v>18</v>
+      </c>
+      <c r="G75" s="3">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" t="s">
+        <v>207</v>
+      </c>
+      <c r="E76" t="s">
+        <v>207</v>
+      </c>
+      <c r="F76" s="4">
+        <v>19</v>
+      </c>
+      <c r="G76" s="3">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" t="s">
+        <v>138</v>
+      </c>
+      <c r="D77" t="s">
+        <v>207</v>
+      </c>
+      <c r="E77" t="s">
+        <v>207</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" t="s">
+        <v>207</v>
+      </c>
+      <c r="E78" t="s">
+        <v>207</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" t="s">
+        <v>207</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G79" s="3">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" t="s">
+        <v>142</v>
+      </c>
+      <c r="D80" t="s">
+        <v>207</v>
+      </c>
+      <c r="E80" t="s">
+        <v>207</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G80" s="3">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81" t="s">
+        <v>207</v>
+      </c>
+      <c r="E81" t="s">
+        <v>207</v>
+      </c>
+      <c r="F81" s="4">
+        <v>10</v>
+      </c>
+      <c r="G81" s="3">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>144</v>
+      </c>
+      <c r="C82" t="s">
+        <v>145</v>
+      </c>
+      <c r="D82" t="s">
+        <v>207</v>
+      </c>
+      <c r="E82" t="s">
+        <v>207</v>
+      </c>
+      <c r="F82" s="4">
+        <v>11</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83" t="s">
+        <v>146</v>
+      </c>
+      <c r="D83" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" s="3">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>147</v>
+      </c>
+      <c r="C84" t="s">
+        <v>148</v>
+      </c>
+      <c r="D84" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" t="s">
+        <v>207</v>
+      </c>
+      <c r="G84" s="3">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>149</v>
+      </c>
+      <c r="C85" t="s">
+        <v>150</v>
+      </c>
+      <c r="D85" t="s">
+        <v>207</v>
+      </c>
+      <c r="E85" t="s">
+        <v>207</v>
+      </c>
+      <c r="G85" s="3">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>151</v>
+      </c>
+      <c r="C86" t="s">
+        <v>152</v>
+      </c>
+      <c r="D86" t="s">
+        <v>207</v>
+      </c>
+      <c r="E86" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" s="3">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>153</v>
+      </c>
+      <c r="C87" t="s">
+        <v>154</v>
+      </c>
+      <c r="D87" t="s">
+        <v>207</v>
+      </c>
+      <c r="E87" t="s">
+        <v>207</v>
+      </c>
+      <c r="G87" s="3">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>155</v>
+      </c>
+      <c r="C88" t="s">
+        <v>155</v>
+      </c>
+      <c r="E88" t="s">
+        <v>207</v>
+      </c>
+      <c r="F88" t="s">
+        <v>155</v>
+      </c>
+      <c r="G88" s="3">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" t="s">
+        <v>156</v>
+      </c>
+      <c r="E89" t="s">
+        <v>207</v>
+      </c>
+      <c r="F89" t="s">
+        <v>156</v>
+      </c>
+      <c r="G89" s="3">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" t="s">
+        <v>157</v>
+      </c>
+      <c r="E90" t="s">
+        <v>207</v>
+      </c>
+      <c r="F90" s="4">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>158</v>
+      </c>
+      <c r="C91" t="s">
+        <v>158</v>
+      </c>
+      <c r="E91" t="s">
+        <v>207</v>
+      </c>
+      <c r="F91" s="4">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" t="s">
+        <v>160</v>
+      </c>
+      <c r="D92" t="s">
+        <v>207</v>
+      </c>
+      <c r="E92" t="s">
+        <v>207</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" t="s">
+        <v>162</v>
+      </c>
+      <c r="D93" t="s">
+        <v>207</v>
+      </c>
+      <c r="E93" t="s">
+        <v>207</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" t="s">
+        <v>164</v>
+      </c>
+      <c r="D94" t="s">
+        <v>207</v>
+      </c>
+      <c r="E94" t="s">
+        <v>207</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" t="s">
+        <v>166</v>
+      </c>
+      <c r="D95" t="s">
+        <v>207</v>
+      </c>
+      <c r="E95" t="s">
+        <v>207</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="G95" s="3">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" t="s">
+        <v>167</v>
+      </c>
+      <c r="G96" s="1">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" t="s">
+        <v>168</v>
+      </c>
+      <c r="G97" s="1">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>169</v>
+      </c>
+      <c r="C98" t="s">
+        <v>170</v>
+      </c>
+      <c r="D98" t="s">
+        <v>207</v>
+      </c>
+      <c r="E98" t="s">
+        <v>207</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G98" s="3">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>171</v>
+      </c>
+      <c r="C99" t="s">
+        <v>172</v>
+      </c>
+      <c r="D99" t="s">
+        <v>207</v>
+      </c>
+      <c r="E99" t="s">
+        <v>207</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="G99" s="3">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>173</v>
+      </c>
+      <c r="C100" t="s">
+        <v>174</v>
+      </c>
+      <c r="D100" t="s">
+        <v>207</v>
+      </c>
+      <c r="E100" t="s">
+        <v>207</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" t="s">
+        <v>176</v>
+      </c>
+      <c r="D101" t="s">
+        <v>207</v>
+      </c>
+      <c r="E101" t="s">
+        <v>207</v>
+      </c>
+      <c r="G101" s="3">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>177</v>
+      </c>
+      <c r="C102" t="s">
+        <v>178</v>
+      </c>
+      <c r="D102" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" t="s">
+        <v>207</v>
+      </c>
+      <c r="G102" s="3">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" t="s">
+        <v>179</v>
+      </c>
+      <c r="D103" t="s">
+        <v>207</v>
+      </c>
+      <c r="E103" t="s">
+        <v>207</v>
+      </c>
+      <c r="G103" s="3">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" t="s">
+        <v>181</v>
+      </c>
+      <c r="G104" s="1">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>182</v>
+      </c>
+      <c r="C105" t="s">
+        <v>183</v>
+      </c>
+      <c r="G105" s="1">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" t="s">
+        <v>185</v>
+      </c>
+      <c r="G106" s="1">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>186</v>
+      </c>
+      <c r="C107" t="s">
+        <v>186</v>
+      </c>
+      <c r="G107" s="1">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>187</v>
+      </c>
+      <c r="C108" t="s">
+        <v>188</v>
+      </c>
+      <c r="G108" s="1">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>189</v>
+      </c>
+      <c r="C109" t="s">
+        <v>190</v>
+      </c>
+      <c r="G109" s="1">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" t="s">
+        <v>192</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" t="s">
+        <v>194</v>
+      </c>
+      <c r="G111" s="1">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>195</v>
+      </c>
+      <c r="C112" t="s">
+        <v>196</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>197</v>
+      </c>
+      <c r="C113" t="s">
+        <v>198</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>199</v>
+      </c>
+      <c r="C114" t="s">
+        <v>199</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>200</v>
+      </c>
+      <c r="C115" t="s">
+        <v>200</v>
+      </c>
+      <c r="G115" s="1">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>201</v>
+      </c>
+      <c r="C116" t="s">
+        <v>201</v>
+      </c>
+      <c r="G116" s="1">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>202</v>
+      </c>
+      <c r="C117" t="s">
+        <v>202</v>
+      </c>
+      <c r="G117" s="1">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>203</v>
+      </c>
+      <c r="C118" t="s">
+        <v>203</v>
+      </c>
+      <c r="G118" s="1">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>204</v>
+      </c>
+      <c r="C119" t="s">
+        <v>204</v>
+      </c>
+      <c r="G119" s="1">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>205</v>
+      </c>
+      <c r="C120" t="s">
+        <v>205</v>
+      </c>
+      <c r="G120" s="1">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>206</v>
+      </c>
+      <c r="C121" t="s">
+        <v>206</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update a faster IgBlast parser(not finished)
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6863D891-5C07-DD4F-9574-ECBC2321449A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ECEAA8-9560-FD49-A58F-BE68529384B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="4800" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="15380" yWindow="4760" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
     <sheet name="IMGT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="250">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -748,72 +748,15 @@
     <t>IgBlast FMT 19</t>
   </si>
   <si>
-    <t>74-62</t>
-  </si>
-  <si>
-    <t>75-62</t>
-  </si>
-  <si>
-    <t>77-62</t>
-  </si>
-  <si>
-    <t>76-62</t>
-  </si>
-  <si>
-    <t>78-62</t>
-  </si>
-  <si>
-    <t>79-62</t>
-  </si>
-  <si>
-    <t>80-62</t>
-  </si>
-  <si>
-    <t>81-62</t>
-  </si>
-  <si>
-    <t>82-62</t>
-  </si>
-  <si>
-    <t>83-62</t>
-  </si>
-  <si>
-    <t>75-74</t>
-  </si>
-  <si>
-    <t>77-76</t>
-  </si>
-  <si>
-    <t>79-78</t>
-  </si>
-  <si>
-    <t>81-80</t>
-  </si>
-  <si>
-    <t>83-82</t>
-  </si>
-  <si>
-    <t>cmp 10 and 11</t>
-  </si>
-  <si>
     <t>IgBlast FMT 3</t>
   </si>
   <si>
     <t>V-(D)-J junction</t>
   </si>
   <si>
-    <t>j begin - v end</t>
-  </si>
-  <si>
-    <t>V-(D)-J rearrangement</t>
-  </si>
-  <si>
     <t>Alignments</t>
   </si>
   <si>
-    <t>cmp 12 and 13</t>
-  </si>
-  <si>
     <t>'</t>
   </si>
   <si>
@@ -824,6 +767,15 @@
   </si>
   <si>
     <t>j1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequences producing significant alignments: </t>
+  </si>
+  <si>
+    <t>Alignment summary</t>
+  </si>
+  <si>
+    <t>later</t>
   </si>
 </sst>
 </file>
@@ -4139,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4164,7 +4116,7 @@
         <v>213</v>
       </c>
       <c r="H1" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4183,7 +4135,7 @@
       <c r="E2" t="s">
         <v>207</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="3">
@@ -4207,7 +4159,7 @@
       <c r="E3" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="3">
@@ -4231,7 +4183,7 @@
       <c r="E4" t="s">
         <v>207</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="3">
@@ -4255,12 +4207,12 @@
       <c r="E5" t="s">
         <v>207</v>
       </c>
-      <c r="F5" s="4">
-        <v>7</v>
-      </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -4279,12 +4231,12 @@
       <c r="E6" t="s">
         <v>207</v>
       </c>
-      <c r="F6" s="4">
-        <v>7</v>
-      </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -4303,12 +4255,12 @@
       <c r="E7" t="s">
         <v>207</v>
       </c>
-      <c r="F7" s="4">
-        <v>7</v>
-      </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -4327,12 +4279,12 @@
       <c r="E8" t="s">
         <v>207</v>
       </c>
-      <c r="F8" s="4">
-        <v>8</v>
-      </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4351,12 +4303,12 @@
       <c r="E9" t="s">
         <v>207</v>
       </c>
-      <c r="F9" s="4">
-        <v>8</v>
-      </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4375,12 +4327,12 @@
       <c r="E10" t="s">
         <v>207</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
+      <c r="H10" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -4399,12 +4351,12 @@
       <c r="E11" t="s">
         <v>207</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="3">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+      <c r="H11" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4423,12 +4375,12 @@
       <c r="E12" t="s">
         <v>207</v>
       </c>
-      <c r="F12" s="4">
-        <v>9</v>
-      </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -4447,12 +4399,12 @@
       <c r="E13" t="s">
         <v>207</v>
       </c>
-      <c r="F13" s="4">
-        <v>9</v>
-      </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -4471,10 +4423,10 @@
       <c r="E14" t="s">
         <v>207</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="3">
         <v>12</v>
       </c>
     </row>
@@ -4494,7 +4446,7 @@
       <c r="E15" t="s">
         <v>207</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="2">
         <v>4</v>
       </c>
       <c r="G15" s="3">
@@ -4518,7 +4470,7 @@
       <c r="E16" t="s">
         <v>207</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="2">
         <v>5</v>
       </c>
       <c r="G16" s="3">
@@ -4542,13 +4494,14 @@
       <c r="E17" t="s">
         <v>207</v>
       </c>
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>259</v>
-      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -4570,8 +4523,8 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H18" t="s">
-        <v>257</v>
+      <c r="H18" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -4594,8 +4547,8 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H19" t="s">
-        <v>257</v>
+      <c r="H19" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4618,8 +4571,8 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H20" t="s">
-        <v>257</v>
+      <c r="H20" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -4642,8 +4595,8 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H21" t="s">
-        <v>257</v>
+      <c r="H21" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -4666,8 +4619,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H22" t="s">
-        <v>257</v>
+      <c r="H22" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -4686,12 +4639,12 @@
       <c r="E23" t="s">
         <v>210</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>258</v>
-      </c>
       <c r="G23" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -4710,12 +4663,12 @@
       <c r="E24" t="s">
         <v>207</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>240</v>
-      </c>
       <c r="G24" s="3">
         <f t="shared" si="0"/>
         <v>22</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -4734,12 +4687,12 @@
       <c r="E25" t="s">
         <v>207</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>241</v>
-      </c>
       <c r="G25" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -4758,12 +4711,12 @@
       <c r="E26" t="s">
         <v>207</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="G26" s="3">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -4782,12 +4735,12 @@
       <c r="E27" t="s">
         <v>207</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -4806,12 +4759,12 @@
       <c r="E28" t="s">
         <v>207</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G28" s="3">
         <f t="shared" si="0"/>
         <v>26</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -4830,12 +4783,12 @@
       <c r="E29" t="s">
         <v>207</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G29" s="3">
         <f t="shared" si="0"/>
         <v>27</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4854,12 +4807,12 @@
       <c r="E30" t="s">
         <v>207</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G30" s="3">
         <f t="shared" si="0"/>
         <v>28</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -4878,12 +4831,12 @@
       <c r="E31" t="s">
         <v>207</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="G31" s="3">
         <f t="shared" si="0"/>
         <v>29</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -4902,15 +4855,15 @@
       <c r="E32" t="s">
         <v>207</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="G32" s="3">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4926,15 +4879,15 @@
       <c r="E33" t="s">
         <v>207</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>251</v>
-      </c>
       <c r="G33" s="3">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4950,15 +4903,15 @@
       <c r="E34" t="s">
         <v>207</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G34" s="3">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4974,15 +4927,15 @@
       <c r="E35" t="s">
         <v>207</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G35" s="3">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4998,15 +4951,15 @@
       <c r="E36" t="s">
         <v>207</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G36" s="3">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5022,15 +4975,15 @@
       <c r="E37" t="s">
         <v>207</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G37" s="3">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5046,15 +4999,15 @@
       <c r="E38" t="s">
         <v>207</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="G38" s="3">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5070,15 +5023,15 @@
       <c r="E39" t="s">
         <v>207</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>245</v>
-      </c>
       <c r="G39" s="3">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5094,15 +5047,15 @@
       <c r="E40" t="s">
         <v>207</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>252</v>
-      </c>
       <c r="G40" s="3">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5118,15 +5071,15 @@
       <c r="E41" t="s">
         <v>207</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G41" s="3">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5142,15 +5095,15 @@
       <c r="E42" t="s">
         <v>207</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G42" s="3">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5166,15 +5119,15 @@
       <c r="E43" t="s">
         <v>207</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G43" s="3">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5190,15 +5143,15 @@
       <c r="E44" t="s">
         <v>207</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G44" s="3">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5214,15 +5167,15 @@
       <c r="E45" t="s">
         <v>207</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>246</v>
-      </c>
       <c r="G45" s="3">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5238,15 +5191,15 @@
       <c r="E46" t="s">
         <v>207</v>
       </c>
-      <c r="F46" s="4" t="s">
-        <v>247</v>
-      </c>
       <c r="G46" s="3">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5262,15 +5215,15 @@
       <c r="E47" t="s">
         <v>207</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>253</v>
-      </c>
       <c r="G47" s="3">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5286,12 +5239,12 @@
       <c r="E48" t="s">
         <v>207</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G48" s="3">
         <f t="shared" si="0"/>
         <v>46</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -5310,12 +5263,12 @@
       <c r="E49" t="s">
         <v>207</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G49" s="3">
         <f t="shared" si="0"/>
         <v>47</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -5334,12 +5287,12 @@
       <c r="E50" t="s">
         <v>207</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G50" s="3">
         <f t="shared" si="0"/>
         <v>48</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -5358,12 +5311,12 @@
       <c r="E51" t="s">
         <v>207</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G51" s="3">
         <f t="shared" si="0"/>
         <v>49</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -5382,12 +5335,12 @@
       <c r="E52" t="s">
         <v>207</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="G52" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -5406,12 +5359,12 @@
       <c r="E53" t="s">
         <v>207</v>
       </c>
-      <c r="F53" s="4" t="s">
-        <v>249</v>
-      </c>
       <c r="G53" s="3">
         <f t="shared" si="0"/>
         <v>51</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -5430,12 +5383,12 @@
       <c r="E54" t="s">
         <v>207</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>254</v>
-      </c>
       <c r="G54" s="3">
         <f t="shared" si="0"/>
         <v>52</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -5454,12 +5407,12 @@
       <c r="E55" t="s">
         <v>207</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G55" s="3">
         <f t="shared" si="0"/>
         <v>53</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -5478,12 +5431,12 @@
       <c r="E56" t="s">
         <v>207</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G56" s="3">
         <f t="shared" si="0"/>
         <v>54</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -5502,12 +5455,12 @@
       <c r="E57" t="s">
         <v>207</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G57" s="3">
         <f t="shared" si="0"/>
         <v>55</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -5526,12 +5479,12 @@
       <c r="E58" t="s">
         <v>207</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>255</v>
-      </c>
       <c r="G58" s="3">
         <f t="shared" si="0"/>
         <v>56</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -5551,11 +5504,14 @@
         <v>207</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="0"/>
         <v>57</v>
+      </c>
+      <c r="H59" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -5575,8 +5531,8 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="H60" t="s">
-        <v>260</v>
+      <c r="H60" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -5692,7 +5648,7 @@
         <v>207</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="G65" s="3">
         <f t="shared" si="0"/>
@@ -5716,7 +5672,7 @@
         <v>207</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="G66" s="3">
         <f t="shared" si="0"/>
@@ -5884,7 +5840,7 @@
         <v>207</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="G73" s="3">
         <f t="shared" si="1"/>
@@ -5908,7 +5864,7 @@
         <v>207</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="G74" s="3">
         <f t="shared" si="1"/>
@@ -6059,7 +6015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6083,7 +6039,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6107,7 +6063,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6128,7 +6084,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6149,7 +6105,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6170,7 +6126,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6191,7 +6147,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6212,7 +6168,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6233,7 +6189,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6254,7 +6210,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6275,7 +6231,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6296,7 +6252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6312,15 +6268,15 @@
       <c r="E92" t="s">
         <v>207</v>
       </c>
-      <c r="F92" s="4" t="s">
-        <v>263</v>
-      </c>
       <c r="G92" s="3">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6336,15 +6292,15 @@
       <c r="E93" t="s">
         <v>207</v>
       </c>
-      <c r="F93" s="4" t="s">
-        <v>264</v>
-      </c>
       <c r="G93" s="3">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6360,15 +6316,15 @@
       <c r="E94" t="s">
         <v>207</v>
       </c>
-      <c r="F94" s="4" t="s">
-        <v>265</v>
-      </c>
       <c r="G94" s="3">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6392,7 +6348,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6407,7 +6363,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6422,7 +6378,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6439,14 +6395,14 @@
         <v>207</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="G98" s="3">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6463,14 +6419,14 @@
         <v>207</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="G99" s="3">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6490,8 +6446,11 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6511,8 +6470,11 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6532,8 +6494,11 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6553,8 +6518,11 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6569,7 +6537,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6584,7 +6552,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6599,7 +6567,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6614,7 +6582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -6629,7 +6597,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -6644,7 +6612,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -6659,7 +6627,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -6674,7 +6642,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -6829,5 +6797,6 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update a fast version to import IgBlast
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ECEAA8-9560-FD49-A58F-BE68529384B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0FEA5F-96E6-D441-A1C3-39189C15448A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15380" yWindow="4760" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="250">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -833,7 +833,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4091,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25:H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5551,7 +5551,7 @@
       <c r="E61" t="s">
         <v>207</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="2">
         <v>64</v>
       </c>
       <c r="G61" s="3">
@@ -5575,7 +5575,7 @@
       <c r="E62" t="s">
         <v>207</v>
       </c>
-      <c r="F62" s="4">
+      <c r="F62" s="2">
         <v>65</v>
       </c>
       <c r="G62" s="3">
@@ -5599,7 +5599,7 @@
       <c r="E63" t="s">
         <v>207</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="2">
         <v>68</v>
       </c>
       <c r="G63" s="3">
@@ -5623,7 +5623,7 @@
       <c r="E64" t="s">
         <v>207</v>
       </c>
-      <c r="F64" s="4">
+      <c r="F64" s="2">
         <v>69</v>
       </c>
       <c r="G64" s="3">
@@ -5695,7 +5695,7 @@
       <c r="E67" t="s">
         <v>207</v>
       </c>
-      <c r="F67" s="4">
+      <c r="F67" s="2">
         <v>72</v>
       </c>
       <c r="G67" s="3">
@@ -5719,7 +5719,7 @@
       <c r="E68" t="s">
         <v>207</v>
       </c>
-      <c r="F68" s="4">
+      <c r="F68" s="2">
         <v>73</v>
       </c>
       <c r="G68" s="3">
@@ -5743,7 +5743,7 @@
       <c r="E69" t="s">
         <v>207</v>
       </c>
-      <c r="F69" s="4">
+      <c r="F69" s="2">
         <v>14</v>
       </c>
       <c r="G69" s="3">
@@ -5767,7 +5767,7 @@
       <c r="E70" t="s">
         <v>207</v>
       </c>
-      <c r="F70" s="4">
+      <c r="F70" s="2">
         <v>15</v>
       </c>
       <c r="G70" s="3">
@@ -5791,7 +5791,7 @@
       <c r="E71" t="s">
         <v>207</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="2">
         <v>16</v>
       </c>
       <c r="G71" s="3">
@@ -5815,7 +5815,7 @@
       <c r="E72" t="s">
         <v>207</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="2">
         <v>17</v>
       </c>
       <c r="G72" s="3">
@@ -5887,7 +5887,7 @@
       <c r="E75" t="s">
         <v>207</v>
       </c>
-      <c r="F75" s="4">
+      <c r="F75" s="2">
         <v>18</v>
       </c>
       <c r="G75" s="3">
@@ -5911,7 +5911,7 @@
       <c r="E76" t="s">
         <v>207</v>
       </c>
-      <c r="F76" s="4">
+      <c r="F76" s="2">
         <v>19</v>
       </c>
       <c r="G76" s="3">
@@ -6031,7 +6031,7 @@
       <c r="E81" t="s">
         <v>207</v>
       </c>
-      <c r="F81" s="4">
+      <c r="F81" s="2">
         <v>10</v>
       </c>
       <c r="G81" s="3">
@@ -6055,7 +6055,7 @@
       <c r="E82" t="s">
         <v>207</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="2">
         <v>11</v>
       </c>
       <c r="G82" s="1">
@@ -6079,6 +6079,9 @@
       <c r="E83" t="s">
         <v>207</v>
       </c>
+      <c r="F83" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G83" s="3">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -6100,6 +6103,9 @@
       <c r="E84" t="s">
         <v>207</v>
       </c>
+      <c r="F84" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G84" s="3">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -6121,6 +6127,9 @@
       <c r="E85" t="s">
         <v>207</v>
       </c>
+      <c r="F85" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G85" s="3">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -6142,6 +6151,9 @@
       <c r="E86" t="s">
         <v>207</v>
       </c>
+      <c r="F86" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G86" s="3">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -6163,6 +6175,9 @@
       <c r="E87" t="s">
         <v>207</v>
       </c>
+      <c r="F87" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G87" s="3">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -6181,7 +6196,7 @@
       <c r="E88" t="s">
         <v>207</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="2" t="s">
         <v>155</v>
       </c>
       <c r="G88" s="3">
@@ -6202,7 +6217,7 @@
       <c r="E89" t="s">
         <v>207</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="2" t="s">
         <v>156</v>
       </c>
       <c r="G89" s="3">
@@ -6223,7 +6238,7 @@
       <c r="E90" t="s">
         <v>207</v>
       </c>
-      <c r="F90" s="4">
+      <c r="F90" s="2">
         <v>0</v>
       </c>
       <c r="G90" s="3">
@@ -6244,7 +6259,7 @@
       <c r="E91" t="s">
         <v>207</v>
       </c>
-      <c r="F91" s="4">
+      <c r="F91" s="2">
         <v>0</v>
       </c>
       <c r="G91" s="3">
@@ -6340,7 +6355,7 @@
       <c r="E95" t="s">
         <v>207</v>
       </c>
-      <c r="F95" s="4" t="s">
+      <c r="F95" s="2" t="s">
         <v>231</v>
       </c>
       <c r="G95" s="3">
@@ -6466,13 +6481,14 @@
       <c r="E101" t="s">
         <v>207</v>
       </c>
+      <c r="F101" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G101" s="3">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="H101" s="4" t="s">
-        <v>236</v>
-      </c>
+      <c r="H101" s="4"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102">
@@ -6490,13 +6506,14 @@
       <c r="E102" t="s">
         <v>207</v>
       </c>
+      <c r="F102" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="G102" s="3">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H102" s="4" t="s">
-        <v>236</v>
-      </c>
+      <c r="H102" s="4"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103">

</xml_diff>

<commit_message>
Fix fast mode in "import" function
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7AB4C8-2A6F-3F42-8E35-266979D5C73C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9CE290-BC0F-C344-B3A2-90BC1C68049B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15380" yWindow="4760" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
@@ -830,10 +830,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,11 +1166,11 @@
       <c r="D1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="1" t="s">
         <v>213</v>
       </c>
@@ -4091,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4108,10 +4108,10 @@
       <c r="D1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="1" t="s">
         <v>213</v>
       </c>
@@ -5647,7 +5647,7 @@
       <c r="E65" t="s">
         <v>207</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G65" s="3">
@@ -5671,7 +5671,7 @@
       <c r="E66" t="s">
         <v>207</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G66" s="3">
@@ -5839,7 +5839,7 @@
       <c r="E73" t="s">
         <v>207</v>
       </c>
-      <c r="F73" s="6" t="s">
+      <c r="F73" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G73" s="3">
@@ -5863,7 +5863,7 @@
       <c r="E74" t="s">
         <v>207</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="F74" s="5" t="s">
         <v>243</v>
       </c>
       <c r="G74" s="3">

</xml_diff>

<commit_message>
Update import igblast function
1) update import igblast function (fmt19)
2) update Vstart and Jend display
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9CE290-BC0F-C344-B3A2-90BC1C68049B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7957AC36-F4B5-8D4B-AF89-1F877F4F6705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="4760" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="5120" yWindow="3780" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
     <sheet name="IMGT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="251">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -745,9 +745,6 @@
     <t>6 pr 7</t>
   </si>
   <si>
-    <t>IgBlast FMT 19</t>
-  </si>
-  <si>
     <t>IgBlast FMT 3</t>
   </si>
   <si>
@@ -776,6 +773,12 @@
   </si>
   <si>
     <t>later</t>
+  </si>
+  <si>
+    <t>IgBlast FMT 19*</t>
+  </si>
+  <si>
+    <t>* igblast new version, added a col at 9. So all number &gt; 9 should be + 1</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1CAC7E-D6FA-A445-AE9E-B41AFE7C83FC}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F98" sqref="F98:G103"/>
     </sheetView>
   </sheetViews>
@@ -4089,10 +4092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="B114" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4109,14 +4112,14 @@
         <v>208</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="1" t="s">
         <v>213</v>
       </c>
       <c r="H1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4212,7 +4215,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -4236,7 +4239,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -4260,7 +4263,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -4284,7 +4287,7 @@
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -4308,7 +4311,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -4332,7 +4335,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -4356,7 +4359,7 @@
         <v>9</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -4380,7 +4383,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -4404,7 +4407,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -4524,7 +4527,7 @@
         <v>16</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -4548,7 +4551,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -4572,7 +4575,7 @@
         <v>18</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -4596,7 +4599,7 @@
         <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -4620,7 +4623,7 @@
         <v>20</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -4644,7 +4647,7 @@
         <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -4668,7 +4671,7 @@
         <v>22</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -4692,7 +4695,7 @@
         <v>23</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -4716,7 +4719,7 @@
         <v>24</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -4740,7 +4743,7 @@
         <v>25</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -4764,7 +4767,7 @@
         <v>26</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -4788,7 +4791,7 @@
         <v>27</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -4812,7 +4815,7 @@
         <v>28</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -4836,7 +4839,7 @@
         <v>29</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -4860,7 +4863,7 @@
         <v>30</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -4884,7 +4887,7 @@
         <v>31</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -4908,7 +4911,7 @@
         <v>32</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -4932,7 +4935,7 @@
         <v>33</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -4956,7 +4959,7 @@
         <v>34</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -4980,7 +4983,7 @@
         <v>35</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -5004,7 +5007,7 @@
         <v>36</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -5028,7 +5031,7 @@
         <v>37</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -5052,7 +5055,7 @@
         <v>38</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -5076,7 +5079,7 @@
         <v>39</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -5100,7 +5103,7 @@
         <v>40</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -5124,7 +5127,7 @@
         <v>41</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -5148,7 +5151,7 @@
         <v>42</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -5172,7 +5175,7 @@
         <v>43</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -5196,7 +5199,7 @@
         <v>44</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -5220,7 +5223,7 @@
         <v>45</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -5244,7 +5247,7 @@
         <v>46</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -5268,7 +5271,7 @@
         <v>47</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -5292,7 +5295,7 @@
         <v>48</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -5316,7 +5319,7 @@
         <v>49</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -5340,7 +5343,7 @@
         <v>50</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -5364,7 +5367,7 @@
         <v>51</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -5388,7 +5391,7 @@
         <v>52</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -5412,7 +5415,7 @@
         <v>53</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -5436,7 +5439,7 @@
         <v>54</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -5460,7 +5463,7 @@
         <v>55</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -5484,7 +5487,7 @@
         <v>56</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -5504,14 +5507,14 @@
         <v>207</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="H59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -5532,7 +5535,7 @@
         <v>58</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -5648,7 +5651,7 @@
         <v>207</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G65" s="3">
         <f t="shared" si="0"/>
@@ -5672,7 +5675,7 @@
         <v>207</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G66" s="3">
         <f t="shared" si="0"/>
@@ -5840,7 +5843,7 @@
         <v>207</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G73" s="3">
         <f t="shared" si="1"/>
@@ -5864,7 +5867,7 @@
         <v>207</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G74" s="3">
         <f t="shared" si="1"/>
@@ -6288,7 +6291,7 @@
         <v>90</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -6312,7 +6315,7 @@
         <v>91</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -6336,7 +6339,7 @@
         <v>92</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -6410,7 +6413,7 @@
         <v>207</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G98" s="3">
         <f t="shared" si="1"/>
@@ -6434,7 +6437,7 @@
         <v>207</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G99" s="3">
         <f t="shared" si="1"/>
@@ -6807,6 +6810,11 @@
       <c r="G121" s="1">
         <f t="shared" si="1"/>
         <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update CDR3 information in importing function
</commit_message>
<xml_diff>
--- a/Fields.xlsx
+++ b/Fields.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leil/Documents/Projects/VGene/VGenes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7957AC36-F4B5-8D4B-AF89-1F877F4F6705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E930FEC4-72FA-2C45-9971-4716EBF636D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="3780" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
+    <workbookView xWindow="2160" yWindow="3620" windowWidth="27300" windowHeight="20760" activeTab="1" xr2:uid="{C65C646D-18C2-4442-A9AB-9139F79DD77F}"/>
   </bookViews>
   <sheets>
     <sheet name="IMGT" sheetId="1" r:id="rId1"/>
     <sheet name="IgBlast" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="345">
   <si>
     <t xml:space="preserve"> "SeqName"</t>
   </si>
@@ -772,13 +773,295 @@
     <t>Alignment summary</t>
   </si>
   <si>
-    <t>later</t>
-  </si>
-  <si>
     <t>IgBlast FMT 19*</t>
   </si>
   <si>
     <t>* igblast new version, added a col at 9. So all number &gt; 9 should be + 1</t>
+  </si>
+  <si>
+    <t>sequence_id</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>locus</t>
+  </si>
+  <si>
+    <t>stop_codon</t>
+  </si>
+  <si>
+    <t>vj_in_frame</t>
+  </si>
+  <si>
+    <t>productive</t>
+  </si>
+  <si>
+    <t>rev_comp</t>
+  </si>
+  <si>
+    <t>complete_vdj</t>
+  </si>
+  <si>
+    <t>v_call</t>
+  </si>
+  <si>
+    <t>d_call</t>
+  </si>
+  <si>
+    <t>j_call</t>
+  </si>
+  <si>
+    <t>sequence_alignment</t>
+  </si>
+  <si>
+    <t>germline_alignment</t>
+  </si>
+  <si>
+    <t>sequence_alignment_aa</t>
+  </si>
+  <si>
+    <t>germline_alignment_aa</t>
+  </si>
+  <si>
+    <t>v_alignment_start</t>
+  </si>
+  <si>
+    <t>v_alignment_end</t>
+  </si>
+  <si>
+    <t>d_alignment_start</t>
+  </si>
+  <si>
+    <t>d_alignment_end</t>
+  </si>
+  <si>
+    <t>j_alignment_start</t>
+  </si>
+  <si>
+    <t>j_alignment_end</t>
+  </si>
+  <si>
+    <t>v_sequence_alignment</t>
+  </si>
+  <si>
+    <t>v_sequence_alignment_aa</t>
+  </si>
+  <si>
+    <t>v_germline_alignment</t>
+  </si>
+  <si>
+    <t>v_germline_alignment_aa</t>
+  </si>
+  <si>
+    <t>d_sequence_alignment</t>
+  </si>
+  <si>
+    <t>d_sequence_alignment_aa</t>
+  </si>
+  <si>
+    <t>d_germline_alignment</t>
+  </si>
+  <si>
+    <t>d_germline_alignment_aa</t>
+  </si>
+  <si>
+    <t>j_sequence_alignment</t>
+  </si>
+  <si>
+    <t>j_sequence_alignment_aa</t>
+  </si>
+  <si>
+    <t>j_germline_alignment</t>
+  </si>
+  <si>
+    <t>j_germline_alignment_aa</t>
+  </si>
+  <si>
+    <t>fwr1</t>
+  </si>
+  <si>
+    <t>fwr1_aa</t>
+  </si>
+  <si>
+    <t>cdr1</t>
+  </si>
+  <si>
+    <t>cdr1_aa</t>
+  </si>
+  <si>
+    <t>fwr2</t>
+  </si>
+  <si>
+    <t>fwr2_aa</t>
+  </si>
+  <si>
+    <t>cdr2</t>
+  </si>
+  <si>
+    <t>cdr2_aa</t>
+  </si>
+  <si>
+    <t>fwr3</t>
+  </si>
+  <si>
+    <t>fwr3_aa</t>
+  </si>
+  <si>
+    <t>fwr4</t>
+  </si>
+  <si>
+    <t>fwr4_aa</t>
+  </si>
+  <si>
+    <t>cdr3</t>
+  </si>
+  <si>
+    <t>cdr3_aa</t>
+  </si>
+  <si>
+    <t>junction</t>
+  </si>
+  <si>
+    <t>junction_length</t>
+  </si>
+  <si>
+    <t>junction_aa</t>
+  </si>
+  <si>
+    <t>junction_aa_length</t>
+  </si>
+  <si>
+    <t>v_score</t>
+  </si>
+  <si>
+    <t>d_score</t>
+  </si>
+  <si>
+    <t>j_score</t>
+  </si>
+  <si>
+    <t>v_cigar</t>
+  </si>
+  <si>
+    <t>d_cigar</t>
+  </si>
+  <si>
+    <t>j_cigar</t>
+  </si>
+  <si>
+    <t>v_support</t>
+  </si>
+  <si>
+    <t>d_support</t>
+  </si>
+  <si>
+    <t>j_support</t>
+  </si>
+  <si>
+    <t>v_identity</t>
+  </si>
+  <si>
+    <t>d_identity</t>
+  </si>
+  <si>
+    <t>j_identity</t>
+  </si>
+  <si>
+    <t>v_sequence_start</t>
+  </si>
+  <si>
+    <t>v_sequence_end</t>
+  </si>
+  <si>
+    <t>v_germline_start</t>
+  </si>
+  <si>
+    <t>v_germline_end</t>
+  </si>
+  <si>
+    <t>d_sequence_start</t>
+  </si>
+  <si>
+    <t>d_sequence_end</t>
+  </si>
+  <si>
+    <t>d_germline_start</t>
+  </si>
+  <si>
+    <t>d_germline_end</t>
+  </si>
+  <si>
+    <t>j_sequence_start</t>
+  </si>
+  <si>
+    <t>j_sequence_end</t>
+  </si>
+  <si>
+    <t>j_germline_start</t>
+  </si>
+  <si>
+    <t>j_germline_end</t>
+  </si>
+  <si>
+    <t>fwr1_start</t>
+  </si>
+  <si>
+    <t>fwr1_end</t>
+  </si>
+  <si>
+    <t>cdr1_start</t>
+  </si>
+  <si>
+    <t>cdr1_end</t>
+  </si>
+  <si>
+    <t>fwr2_start</t>
+  </si>
+  <si>
+    <t>fwr2_end</t>
+  </si>
+  <si>
+    <t>cdr2_start</t>
+  </si>
+  <si>
+    <t>cdr2_end</t>
+  </si>
+  <si>
+    <t>fwr3_start</t>
+  </si>
+  <si>
+    <t>fwr3_end</t>
+  </si>
+  <si>
+    <t>fwr4_start</t>
+  </si>
+  <si>
+    <t>fwr4_end</t>
+  </si>
+  <si>
+    <t>cdr3_start</t>
+  </si>
+  <si>
+    <t>cdr3_end</t>
+  </si>
+  <si>
+    <t>np1</t>
+  </si>
+  <si>
+    <t>np1_length</t>
+  </si>
+  <si>
+    <t>np2</t>
+  </si>
+  <si>
+    <t>np2_length</t>
+  </si>
+  <si>
+    <t>87-63</t>
+  </si>
+  <si>
+    <t>88-63</t>
   </si>
 </sst>
 </file>
@@ -4094,8 +4377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0B5C9-F950-E042-AA4D-042CAFFF11E3}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B114" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4112,7 +4395,7 @@
         <v>208</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="1" t="s">
@@ -5507,7 +5790,7 @@
         <v>207</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="G59" s="3">
         <f t="shared" si="0"/>
@@ -6035,7 +6318,7 @@
         <v>207</v>
       </c>
       <c r="F81" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G81" s="3">
         <f t="shared" si="1"/>
@@ -6059,7 +6342,7 @@
         <v>207</v>
       </c>
       <c r="F82" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G82" s="1">
         <f t="shared" si="1"/>
@@ -6082,8 +6365,8 @@
       <c r="E83" t="s">
         <v>207</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>236</v>
+      <c r="F83" s="2">
+        <v>45</v>
       </c>
       <c r="G83" s="3">
         <f t="shared" si="1"/>
@@ -6106,8 +6389,8 @@
       <c r="E84" t="s">
         <v>207</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>236</v>
+      <c r="F84" s="2">
+        <v>46</v>
       </c>
       <c r="G84" s="3">
         <f t="shared" si="1"/>
@@ -6130,8 +6413,8 @@
       <c r="E85" t="s">
         <v>207</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>236</v>
+      <c r="F85" s="2">
+        <v>46</v>
       </c>
       <c r="G85" s="3">
         <f t="shared" si="1"/>
@@ -6155,7 +6438,7 @@
         <v>207</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>236</v>
+        <v>343</v>
       </c>
       <c r="G86" s="3">
         <f t="shared" si="1"/>
@@ -6179,7 +6462,7 @@
         <v>207</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>236</v>
+        <v>344</v>
       </c>
       <c r="G87" s="3">
         <f t="shared" si="1"/>
@@ -6413,7 +6696,7 @@
         <v>207</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="G98" s="3">
         <f t="shared" si="1"/>
@@ -6437,7 +6720,7 @@
         <v>207</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="G99" s="3">
         <f t="shared" si="1"/>
@@ -6814,7 +7097,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -6824,4 +7107,767 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB7A9CD-B63C-1140-A58A-123F8E153AF4}">
+  <dimension ref="A1:B93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88:B89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>